<commit_message>
RDCC-2510: updating integration tests
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/Staff Data Upload With Case Insensitive Email.xlsx
+++ b/src/integrationTest/resources/Staff Data Upload With Case Insensitive Email.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/m_900458/Documents/HMCTS/rd-caseworker-ref-api/src/integrationTest/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF586532-35F3-E74A-93AA-909B9F843B3C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04B6516-5151-9242-B70E-0505EAB66644}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16460" activeTab="2" xr2:uid="{C3779BBE-D7A5-4756-9223-DEADF9C5B8AB}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1870" uniqueCount="1204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1859" uniqueCount="1201">
   <si>
     <t>Region</t>
   </si>
@@ -3638,16 +3638,7 @@
     <t>test</t>
   </si>
   <si>
-    <t>test1</t>
-  </si>
-  <si>
-    <t>test2</t>
-  </si>
-  <si>
-    <t>CRDtest-1@JUSTICE.GOV.UK</t>
-  </si>
-  <si>
-    <t>CRDtest-2@justice.gov.uk</t>
+    <t>test-CRD@JUSTICE.GOV.UK</t>
   </si>
 </sst>
 </file>
@@ -7646,7 +7637,7 @@
   <dimension ref="A1:AD50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7783,21 +7774,21 @@
         <v>1199</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>1202</v>
+        <v>1200</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E2" s="1">
         <f>IF(ISNA(VLOOKUP(D2,Region!$A$2:$B$11,2)),"",VLOOKUP(D2,Region!$A$2:$B$11,2))</f>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F2" s="41" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="G2" s="1">
         <f>IF(ISNA(VLOOKUP(F2,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F2,'Base Locations'!$A$1:$F$341,2))</f>
-        <v>827534</v>
+        <v>817181</v>
       </c>
       <c r="H2" s="41" t="s">
         <v>72</v>
@@ -7814,11 +7805,11 @@
       </c>
       <c r="L2" s="41"/>
       <c r="M2" s="41" t="s">
-        <v>1171</v>
+        <v>13</v>
       </c>
       <c r="N2" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M2,Services!$A$1:$B$45,2)),"",VLOOKUP(M2,Services!$A$1:$B$45,2))</f>
-        <v>BHA3</v>
+        <v>BAB1</v>
       </c>
       <c r="O2" s="41"/>
       <c r="P2" s="1" t="str">
@@ -7856,54 +7847,34 @@
         <v/>
       </c>
       <c r="AC2" s="41"/>
-      <c r="AD2" s="41" t="s">
-        <v>1121</v>
-      </c>
+      <c r="AD2" s="41"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A3" s="41" t="s">
-        <v>1200</v>
-      </c>
-      <c r="B3" s="41" t="s">
-        <v>1201</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>1203</v>
-      </c>
-      <c r="D3" s="41" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="A3" s="41"/>
+      <c r="B3" s="41"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(D3,Region!$A$2:$B$11,2)),"",VLOOKUP(D3,Region!$A$2:$B$11,2))</f>
-        <v>3</v>
-      </c>
-      <c r="F3" s="41" t="s">
-        <v>76</v>
-      </c>
-      <c r="G3" s="1">
+        <v/>
+      </c>
+      <c r="F3" s="41"/>
+      <c r="G3" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(F3,'Base Locations'!$A$1:$F$341,2)),"",VLOOKUP(F3,'Base Locations'!$A$1:$F$341,2))</f>
-        <v>218723</v>
-      </c>
-      <c r="H3" s="41" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3" s="1">
+        <v/>
+      </c>
+      <c r="H3" s="41"/>
+      <c r="I3" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(H3,'Base Locations'!A2:F342,2)),"",VLOOKUP(H3,'Base Locations'!A2:F342,2))</f>
-        <v>239985</v>
-      </c>
-      <c r="J3" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="K3" s="41" t="s">
-        <v>408</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J3" s="41"/>
+      <c r="K3" s="41"/>
       <c r="L3" s="41"/>
-      <c r="M3" s="41" t="s">
-        <v>13</v>
-      </c>
+      <c r="M3" s="41"/>
       <c r="N3" s="1" t="str">
         <f>IF(ISNA(VLOOKUP(M3,Services!$A$1:$B$45,2)),"",VLOOKUP(M3,Services!$A$1:$B$45,2))</f>
-        <v>BAB1</v>
+        <v/>
       </c>
       <c r="O3" s="41"/>
       <c r="P3" s="1" t="str">
@@ -7941,9 +7912,7 @@
         <v/>
       </c>
       <c r="AC3" s="41"/>
-      <c r="AD3" s="41" t="s">
-        <v>1121</v>
-      </c>
+      <c r="AD3" s="41"/>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" s="41"/>

</xml_diff>